<commit_message>
added test suites and cucumber
</commit_message>
<xml_diff>
--- a/src/test/resources/customerdata.xlsx
+++ b/src/test/resources/customerdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\eclipse-workspace\automation-demo\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA664763-83D9-4E6B-8267-06415694C12E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86672872-46EB-47F3-A6BF-B91343095EB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AE5F32BC-A108-4C56-B7A0-C79458B805F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{AE5F32BC-A108-4C56-B7A0-C79458B805F5}"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F8B957-03C0-423E-B3EB-7CE4912161E6}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,10 +619,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D07C4A-9D4F-4DE0-BB2C-7EBC22884EA9}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,6 +690,46 @@
         <v>27</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>